<commit_message>
updated LTC for AF
</commit_message>
<xml_diff>
--- a/data-raw/paygrades.xlsx
+++ b/data-raw/paygrades.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bjorn\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\IR&amp;D\IR21-03 HMA Improvements\R\dataOPS\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,7 +1173,7 @@
         <v>66</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C49" t="s">
         <v>25</v>

</xml_diff>